<commit_message>
correct alcohol frequency harmo rule
</commit_message>
<xml_diff>
--- a/data_processing_elements-ERC.xlsx
+++ b/data_processing_elements-ERC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023BC444-5F30-4763-A324-7E4C8B3099E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D1D5B0-14CF-4372-9D54-5EDDB06CE5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1859,9 +1859,6 @@
     <t>Wording is: During the past 12 months, how often have you had alcoholic beverages?</t>
   </si>
   <si>
-    <t>recode(1=3; 2=3; 3=2; 4=2; 6=1; 7=0; 8=0; 9=0; 10=NA; ELSE=NA)</t>
-  </si>
-  <si>
     <t>cig/day</t>
   </si>
   <si>
@@ -1880,6 +1877,9 @@
   </si>
   <si>
     <t>w23gg08</t>
+  </si>
+  <si>
+    <t>recode(1=3; 2=3; 3=2; 4=2;5=1; 6=1; 7=0; 8=0; 9=0; 10=NA; ELSE=NA)</t>
   </si>
 </sst>
 </file>
@@ -2337,10 +2337,10 @@
   <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T18" sqref="T18"/>
+      <selection pane="bottomRight" activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="11" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>295</v>
@@ -4311,7 +4311,7 @@
         <v>32</v>
       </c>
       <c r="S38" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="38.25" x14ac:dyDescent="0.25">
@@ -4384,7 +4384,7 @@
       <c r="H40" s="3"/>
       <c r="I40" s="8"/>
       <c r="J40" s="11" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K40" s="11" t="s">
         <v>380</v>
@@ -4610,7 +4610,7 @@
         <v>39</v>
       </c>
       <c r="S44" s="3" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
     </row>
     <row r="45" spans="1:19" ht="89.25" x14ac:dyDescent="0.25">
@@ -4750,7 +4750,7 @@
       </c>
       <c r="M47" s="8"/>
       <c r="N47" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="O47" s="3"/>
       <c r="P47" s="3" t="s">
@@ -4763,7 +4763,7 @@
         <v>32</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="48" spans="1:19" ht="89.25" x14ac:dyDescent="0.25">
@@ -5144,7 +5144,7 @@
         <v>475</v>
       </c>
       <c r="M55" s="8" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N55" s="3"/>
       <c r="O55" s="3"/>
@@ -5195,7 +5195,7 @@
         <v>476</v>
       </c>
       <c r="M56" s="8" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
@@ -5246,7 +5246,7 @@
         <v>477</v>
       </c>
       <c r="M57" s="8" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N57" s="3"/>
       <c r="O57" s="3"/>

</xml_diff>

<commit_message>
correct value type fruit
</commit_message>
<xml_diff>
--- a/data_processing_elements-ERC.xlsx
+++ b/data_processing_elements-ERC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022C4F3F-0EE1-4F9A-AA14-080873863778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230F5C64-4B0E-4709-BBA3-587EB971AE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -2334,10 +2334,10 @@
   <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q39" sqref="Q39"/>
+      <selection pane="bottomRight" activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4373,7 +4373,7 @@
         <v>159</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
Correct w23date_ent name to w23fecha_ent
</commit_message>
<xml_diff>
--- a/data_processing_elements-ERC.xlsx
+++ b/data_processing_elements-ERC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230F5C64-4B0E-4709-BBA3-587EB971AE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D8A4A2-FDAB-42FA-8F96-81E4264D5038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -1826,12 +1826,6 @@
     <t>During the nurse's visit to the participants' home, they are asked to show all the boxes of medications they regularly consume and the prescriptions, and the nurse writes down all the medications (up to 10 medications). Each recorded medication has been assigned the corresponding ATC code, and this variable has been coded as yes/no based on the list of ATC codes related to antidiabetic medications proposed by PROPASS (see sheet "ATCs_med" in this document).</t>
   </si>
   <si>
-    <t>case_when(
-!is.na(w23date_ent) ~ format(as.Date(w23date_ent, format = "%d/%m/%Y"), "%Y-%m-%d");
-!is.na(w17fecha_ent) ~ format(as.Date(w17fecha_ent, format = "%d/%m/%Y"), "%Y-%m-%d");
-ELSE ~ as.Date(NA))</t>
-  </si>
-  <si>
     <t>recode(1=0; 2=0; 3=0; 4=0; 5=1; 6=3; 7=3; ELSE = NA)</t>
   </si>
   <si>
@@ -1869,14 +1863,20 @@
 1=Yes</t>
   </si>
   <si>
+    <t>w23gg08</t>
+  </si>
+  <si>
+    <t>recode(1=3; 2=3; 3=2; 4=2;5=1; 6=1; 7=0; 8=0; 9=0; 10=NA; ELSE=NA)</t>
+  </si>
+  <si>
     <t>w17fecha_ent;
-w23date_ent</t>
-  </si>
-  <si>
-    <t>w23gg08</t>
-  </si>
-  <si>
-    <t>recode(1=3; 2=3; 3=2; 4=2;5=1; 6=1; 7=0; 8=0; 9=0; 10=NA; ELSE=NA)</t>
+w23fecha_ent</t>
+  </si>
+  <si>
+    <t>case_when(
+!is.na(w23fecha_ent) ~ format(as.Date(w23fecha_ent, format = "%d/%m/%Y"), "%Y-%m-%d");
+!is.na(w17fecha_ent) ~ format(as.Date(w17fecha_ent, format = "%d/%m/%Y"), "%Y-%m-%d");
+ELSE ~ as.Date(NA))</t>
   </si>
 </sst>
 </file>
@@ -2334,10 +2334,10 @@
   <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I43" sqref="I43"/>
+      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2494,7 +2494,7 @@
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="11" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>295</v>
@@ -2517,7 +2517,7 @@
         <v>204</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>478</v>
+        <v>490</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -2672,7 +2672,7 @@
         <v>39</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="127.5" x14ac:dyDescent="0.25">
@@ -3580,7 +3580,7 @@
         <v>32</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -4149,7 +4149,7 @@
         <v>32</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -4381,7 +4381,7 @@
       <c r="H40" s="3"/>
       <c r="I40" s="8"/>
       <c r="J40" s="11" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="K40" s="11" t="s">
         <v>380</v>
@@ -4554,7 +4554,7 @@
         <v>32</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="153" x14ac:dyDescent="0.25">
@@ -4591,11 +4591,11 @@
         <v>473</v>
       </c>
       <c r="M44" s="8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="N44" s="3"/>
       <c r="O44" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="P44" s="3" t="s">
         <v>23</v>
@@ -4607,7 +4607,7 @@
         <v>39</v>
       </c>
       <c r="S44" s="3" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="45" spans="1:19" ht="89.25" x14ac:dyDescent="0.25">
@@ -4747,7 +4747,7 @@
       </c>
       <c r="M47" s="8"/>
       <c r="N47" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="O47" s="3"/>
       <c r="P47" s="3" t="s">
@@ -4760,7 +4760,7 @@
         <v>32</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="48" spans="1:19" ht="89.25" x14ac:dyDescent="0.25">
@@ -5141,7 +5141,7 @@
         <v>475</v>
       </c>
       <c r="M55" s="8" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="N55" s="3"/>
       <c r="O55" s="3"/>
@@ -5192,7 +5192,7 @@
         <v>476</v>
       </c>
       <c r="M56" s="8" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
@@ -5243,7 +5243,7 @@
         <v>477</v>
       </c>
       <c r="M57" s="8" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="N57" s="3"/>
       <c r="O57" s="3"/>

</xml_diff>

<commit_message>
correct adm_date harmo rule
</commit_message>
<xml_diff>
--- a/data_processing_elements-ERC.xlsx
+++ b/data_processing_elements-ERC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D8A4A2-FDAB-42FA-8F96-81E4264D5038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B44CD0E-B6D0-4855-8121-01D6ACD63D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -1874,9 +1874,9 @@
   </si>
   <si>
     <t>case_when(
-!is.na(w23fecha_ent) ~ format(as.Date(w23fecha_ent, format = "%d/%m/%Y"), "%Y-%m-%d");
-!is.na(w17fecha_ent) ~ format(as.Date(w17fecha_ent, format = "%d/%m/%Y"), "%Y-%m-%d");
-ELSE ~ as.Date(NA))</t>
+!is.na(w23fecha_ent) ~ as.character(format(as.Date(w23fecha_ent, format = "%d/%m/%Y"), "%Y-%m-%d"));
+!is.na(w17fecha_ent) ~ as.character(format(as.Date(w17fecha_ent, format = "%d/%m/%Y"), "%Y-%m-%d"));
+ELSE ~ NA)</t>
   </si>
 </sst>
 </file>
@@ -2337,7 +2337,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2469,7 +2469,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="213.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="228" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
correct sdc_employment_description harmo rule
</commit_message>
<xml_diff>
--- a/data_processing_elements-ERC.xlsx
+++ b/data_processing_elements-ERC.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/849507f40a0f895e/Documents/ProPASS/Studies/ENRICA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{9B44CD0E-B6D0-4855-8121-01D6ACD63D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFF4509C-8CF8-4E4C-843E-0F813E0583E8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2791575E-959D-4F06-9FD2-C063B6B6CF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
@@ -1098,29 +1098,6 @@
 99=DK/NA</t>
   </si>
   <si>
-    <t>case_when(
-w23p101 == 1 ~ "Entrepreneur or self-employed worker with 10 or more employees";
-w23p101 == 2 ~ "Entrepreneur or self-employed worker with less than 10 employees";
-w23p101 == 3 ~ "Higher-level self-employed (i.e., Medical doctor, lawyer, psychologist, etc.)";
-w23p101 == 4 ~ "Self-employed medium degree (i.e., nurse, physiotherapist, teacher, etc.)";
-w23p101 == 5 ~ "Self-employed farmer without employees";
-w23p101 == 6 ~ "Other self-employed work without employees";
-w23p101 == 7 ~ "Employed worker: Manager of a company with 10 or more employees";
-w23p101 == 8 ~ "Employed worker: Manager of a company with less than 10 employees";
-w23p101 == 9 ~ "Employed worker: Higher degree (i.e., Medical doctor, lawyer, psychologist, etc.)";
-w23p101 == 10 ~ "Employed worker: Medium degree (i.e., nurse, physical therapist, teacher, etc.)";
-w23p101 == 11 ~ "Employed worker: Supervisor, manager, head of administrative or commercial departments";
-w23p101 == 12 ~ "Employed worker: Other administrative or commercial personnel";
-w23p101 == 13 ~ "Employed worker: Other service personnel";
-w23p101 == 14 ~ "Employed worker: Operators or skilled manual laborers";
-w23p101 == 15 ~ "Employed worker: Semi-skilled and unskilled manual workers or operators";
-w23p101 == 16 ~ "Employed worker: Farmworkers";
-w23p101 == 17 ~ "Employed worker: Armed Forces";
-w23p101 == 18 ~ "Housewife";
-w23p101 == 19 ~ "Others";
-ELSE ~ NA_character_)</t>
-  </si>
-  <si>
     <t>Wording of the category includes "Retired/pensioner".</t>
   </si>
   <si>
@@ -1859,6 +1836,29 @@
 w23p34_18 &gt; 0 | w23p34_14 &gt; 0 | w23p34_15 &gt; 0 | w23p34_16 &gt; 0 | w23p34_17 &gt; 0 | w23p34_19 &gt; 0 ~ 1L;
 w23p34_18 == 0 &amp; w23p34_14 == 0 &amp; w23p34_15 == 0 &amp; w23p34_16 == 0 &amp; w23p34_17 == 0 &amp; w23p34_19 == 0 ~ 0L;
 ELSE ~ NA_integer_)</t>
+  </si>
+  <si>
+    <t>case_when(
+w17p209b == 1 ~ "Entrepreneur or self-employed worker with 10 or more employees";
+w17p209b == 2 ~ "Entrepreneur or self-employed worker with less than 10 employees";
+w17p209b == 3 ~ "Higher-level self-employed (i.e., Medical doctor, lawyer, psychologist, etc.)";
+w17p209b == 4 ~ "Self-employed medium degree (i.e., nurse, physiotherapist, teacher, etc.)";
+w17p209b == 5 ~ "Self-employed farmer without employees";
+w17p209b == 6 ~ "Other self-employed work without employees";
+w17p209b == 7 ~ "Employed worker: Manager of a company with 10 or more employees";
+w17p209b == 8 ~ "Employed worker: Manager of a company with less than 10 employees";
+w17p209b == 9 ~ "Employed worker: Higher degree (i.e., Medical doctor, lawyer, psychologist, etc.)";
+w17p209b == 10 ~ "Employed worker: Medium degree (i.e., nurse, physical therapist, teacher, etc.)";
+w17p209b == 11 ~ "Employed worker: Supervisor, manager, head of administrative or commercial departments";
+w17p209b == 12 ~ "Employed worker: Other administrative or commercial personnel";
+w17p209b == 13 ~ "Employed worker: Other service personnel";
+w17p209b == 14 ~ "Employed worker: Operators or skilled manual laborers";
+w17p209b == 15 ~ "Employed worker: Semi-skilled and unskilled manual workers or operators";
+w17p209b == 16 ~ "Employed worker: Farmworkers";
+w17p209b == 17 ~ "Employed worker: Armed Forces";
+w17p209b == 18 ~ "Housewife";
+w17p209b == 19 ~ "Others";
+ELSE ~ NA_character_)</t>
   </si>
 </sst>
 </file>
@@ -2328,10 +2328,10 @@
   <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K35" sqref="K35"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2488,7 +2488,7 @@
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="11" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>295</v>
@@ -2511,7 +2511,7 @@
         <v>204</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -2666,7 +2666,7 @@
         <v>39</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="127.5" x14ac:dyDescent="0.25">
@@ -2876,7 +2876,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="8"/>
       <c r="J11" s="13" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>312</v>
@@ -2899,7 +2899,7 @@
         <v>204</v>
       </c>
       <c r="S11" s="11" t="s">
-        <v>315</v>
+        <v>488</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="63.75" x14ac:dyDescent="0.25">
@@ -2940,7 +2940,7 @@
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P12" s="3" t="s">
         <v>23</v>
@@ -2952,7 +2952,7 @@
         <v>39</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="76.5" x14ac:dyDescent="0.25">
@@ -2980,16 +2980,16 @@
         <v>79</v>
       </c>
       <c r="J13" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="K13" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="L13" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="M13" s="8" t="s">
         <v>320</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>321</v>
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
@@ -3003,7 +3003,7 @@
         <v>39</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="76.5" x14ac:dyDescent="0.25">
@@ -3031,16 +3031,16 @@
         <v>83</v>
       </c>
       <c r="J14" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="L14" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="M14" s="8" t="s">
         <v>320</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>321</v>
       </c>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
@@ -3127,13 +3127,13 @@
       <c r="H16" s="3"/>
       <c r="I16" s="8"/>
       <c r="J16" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="K16" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="K16" s="11" t="s">
-        <v>324</v>
-      </c>
       <c r="L16" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="M16" s="8" t="s">
         <v>287</v>
@@ -3152,7 +3152,7 @@
         <v>204</v>
       </c>
       <c r="S16" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="114" x14ac:dyDescent="0.25">
@@ -3180,13 +3180,13 @@
         <v>92</v>
       </c>
       <c r="J17" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="K17" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="K17" s="11" t="s">
+      <c r="L17" s="3" t="s">
         <v>324</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>325</v>
       </c>
       <c r="M17" s="8" t="s">
         <v>287</v>
@@ -3205,7 +3205,7 @@
         <v>204</v>
       </c>
       <c r="S17" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="99.75" x14ac:dyDescent="0.25">
@@ -3233,13 +3233,13 @@
       <c r="H18" s="3"/>
       <c r="I18" s="8"/>
       <c r="J18" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="K18" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="K18" s="11" t="s">
+      <c r="L18" s="3" t="s">
         <v>329</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>330</v>
       </c>
       <c r="M18" s="8" t="s">
         <v>287</v>
@@ -3258,7 +3258,7 @@
         <v>204</v>
       </c>
       <c r="S18" s="11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="114" x14ac:dyDescent="0.25">
@@ -3286,13 +3286,13 @@
         <v>92</v>
       </c>
       <c r="J19" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="K19" s="11" t="s">
         <v>328</v>
       </c>
-      <c r="K19" s="11" t="s">
+      <c r="L19" s="3" t="s">
         <v>329</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>330</v>
       </c>
       <c r="M19" s="8" t="s">
         <v>287</v>
@@ -3311,7 +3311,7 @@
         <v>204</v>
       </c>
       <c r="S19" s="11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -3339,13 +3339,13 @@
       <c r="H20" s="3"/>
       <c r="I20" s="8"/>
       <c r="J20" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="K20" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="L20" s="3" t="s">
         <v>334</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>335</v>
       </c>
       <c r="M20" s="8" t="s">
         <v>287</v>
@@ -3392,13 +3392,13 @@
       <c r="H21" s="3"/>
       <c r="I21" s="8"/>
       <c r="J21" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>102</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M21" s="8" t="s">
         <v>287</v>
@@ -3445,13 +3445,13 @@
         <v>92</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>102</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M22" s="8" t="s">
         <v>287</v>
@@ -3470,7 +3470,7 @@
         <v>32</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="42.75" x14ac:dyDescent="0.25">
@@ -3498,19 +3498,19 @@
       <c r="H23" s="3"/>
       <c r="I23" s="8"/>
       <c r="J23" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="K23" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="K23" s="11" t="s">
+      <c r="L23" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="M23" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="M23" s="8" t="s">
+      <c r="N23" s="11" t="s">
         <v>342</v>
-      </c>
-      <c r="N23" s="11" t="s">
-        <v>343</v>
       </c>
       <c r="O23" s="3"/>
       <c r="P23" s="3" t="s">
@@ -3523,7 +3523,7 @@
         <v>32</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="42.75" x14ac:dyDescent="0.25">
@@ -3549,19 +3549,19 @@
       <c r="H24" s="3"/>
       <c r="I24" s="8"/>
       <c r="J24" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="K24" s="11" t="s">
         <v>339</v>
       </c>
-      <c r="K24" s="11" t="s">
+      <c r="L24" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="M24" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="M24" s="8" t="s">
+      <c r="N24" s="11" t="s">
         <v>342</v>
-      </c>
-      <c r="N24" s="11" t="s">
-        <v>343</v>
       </c>
       <c r="O24" s="3"/>
       <c r="P24" s="2" t="s">
@@ -3574,7 +3574,7 @@
         <v>32</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -3602,13 +3602,13 @@
       <c r="H25" s="3"/>
       <c r="I25" s="8"/>
       <c r="J25" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="K25" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="L25" s="3" t="s">
         <v>346</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>347</v>
       </c>
       <c r="M25" s="8" t="s">
         <v>287</v>
@@ -3655,13 +3655,13 @@
       <c r="H26" s="3"/>
       <c r="I26" s="8"/>
       <c r="J26" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="K26" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="L26" s="3" t="s">
         <v>349</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>350</v>
       </c>
       <c r="M26" s="8" t="s">
         <v>287</v>
@@ -3708,13 +3708,13 @@
       <c r="H27" s="3"/>
       <c r="I27" s="8"/>
       <c r="J27" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="K27" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="L27" s="3" t="s">
         <v>352</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>353</v>
       </c>
       <c r="M27" s="8" t="s">
         <v>287</v>
@@ -3851,19 +3851,19 @@
       <c r="H30" s="3"/>
       <c r="I30" s="8"/>
       <c r="J30" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="K30" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="K30" s="3" t="s">
+      <c r="L30" s="3" t="s">
         <v>355</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>356</v>
       </c>
       <c r="M30" s="8" t="s">
         <v>287</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="O30" s="3"/>
       <c r="P30" s="3" t="s">
@@ -3904,13 +3904,13 @@
       <c r="H31" s="3"/>
       <c r="I31" s="8"/>
       <c r="J31" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="K31" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="K31" s="3" t="s">
-        <v>359</v>
-      </c>
       <c r="L31" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="M31" s="8" t="s">
         <v>287</v>
@@ -3957,19 +3957,19 @@
       <c r="H32" s="3"/>
       <c r="I32" s="8"/>
       <c r="J32" s="11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>134</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="M32" s="8" t="s">
         <v>287</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="O32" s="3"/>
       <c r="P32" s="3" t="s">
@@ -3982,7 +3982,7 @@
         <v>32</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -4010,19 +4010,19 @@
       <c r="H33" s="3"/>
       <c r="I33" s="8"/>
       <c r="J33" s="11" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>137</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="M33" s="8" t="s">
         <v>287</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="O33" s="3"/>
       <c r="P33" s="3" t="s">
@@ -4035,7 +4035,7 @@
         <v>32</v>
       </c>
       <c r="S33" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -4063,19 +4063,19 @@
       <c r="H34" s="3"/>
       <c r="I34" s="8"/>
       <c r="J34" s="11" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K34" s="3" t="s">
         <v>139</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="M34" s="8" t="s">
         <v>287</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="O34" s="3"/>
       <c r="P34" s="3" t="s">
@@ -4088,7 +4088,7 @@
         <v>32</v>
       </c>
       <c r="S34" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="42.75" x14ac:dyDescent="0.25">
@@ -4116,19 +4116,19 @@
       <c r="H35" s="3"/>
       <c r="I35" s="8"/>
       <c r="J35" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="K35" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="K35" s="11" t="s">
+      <c r="L35" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="L35" s="3" t="s">
+      <c r="M35" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="M35" s="8" t="s">
+      <c r="N35" s="11" t="s">
         <v>370</v>
-      </c>
-      <c r="N35" s="11" t="s">
-        <v>371</v>
       </c>
       <c r="O35" s="3" t="s">
         <v>288</v>
@@ -4143,7 +4143,7 @@
         <v>32</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -4171,19 +4171,19 @@
       <c r="H36" s="3"/>
       <c r="I36" s="8"/>
       <c r="J36" s="11" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K36" s="3" t="s">
         <v>143</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="M36" s="8" t="s">
         <v>287</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="O36" s="3"/>
       <c r="P36" s="3" t="s">
@@ -4196,7 +4196,7 @@
         <v>32</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -4224,13 +4224,13 @@
       <c r="H37" s="3"/>
       <c r="I37" s="8"/>
       <c r="J37" s="11" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K37" s="3" t="s">
         <v>145</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="M37" s="8" t="s">
         <v>287</v>
@@ -4277,13 +4277,13 @@
       <c r="H38" s="3"/>
       <c r="I38" s="8"/>
       <c r="J38" s="11" t="s">
+        <v>374</v>
+      </c>
+      <c r="K38" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="K38" s="3" t="s">
+      <c r="L38" s="3" t="s">
         <v>376</v>
-      </c>
-      <c r="L38" s="3" t="s">
-        <v>377</v>
       </c>
       <c r="M38" s="8" t="s">
         <v>287</v>
@@ -4375,19 +4375,19 @@
       <c r="H40" s="3"/>
       <c r="I40" s="8"/>
       <c r="J40" s="11" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="K40" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="L40" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="L40" s="3" t="s">
+      <c r="M40" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="N40" s="11" t="s">
         <v>379</v>
-      </c>
-      <c r="M40" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="N40" s="11" t="s">
-        <v>380</v>
       </c>
       <c r="P40" s="3" t="s">
         <v>23</v>
@@ -4472,13 +4472,13 @@
       <c r="H42" s="3"/>
       <c r="I42" s="8"/>
       <c r="J42" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="K42" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="K42" s="3" t="s">
+      <c r="L42" s="3" t="s">
         <v>382</v>
-      </c>
-      <c r="L42" s="3" t="s">
-        <v>383</v>
       </c>
       <c r="M42" s="8" t="s">
         <v>287</v>
@@ -4525,13 +4525,13 @@
       <c r="H43" s="3"/>
       <c r="I43" s="8"/>
       <c r="J43" s="11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="M43" s="8"/>
       <c r="N43" s="3" t="s">
@@ -4548,7 +4548,7 @@
         <v>32</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="153" x14ac:dyDescent="0.25">
@@ -4576,20 +4576,20 @@
         <v>172</v>
       </c>
       <c r="J44" s="11" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="M44" s="8" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="N44" s="3"/>
       <c r="O44" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="P44" s="3" t="s">
         <v>23</v>
@@ -4601,7 +4601,7 @@
         <v>39</v>
       </c>
       <c r="S44" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="45" spans="1:19" ht="89.25" x14ac:dyDescent="0.25">
@@ -4629,16 +4629,16 @@
         <v>176</v>
       </c>
       <c r="J45" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="K45" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="K45" s="3" t="s">
+      <c r="L45" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="L45" s="3" t="s">
+      <c r="M45" s="8" t="s">
         <v>386</v>
-      </c>
-      <c r="M45" s="8" t="s">
-        <v>387</v>
       </c>
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
@@ -4652,7 +4652,7 @@
         <v>39</v>
       </c>
       <c r="S45" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="46" spans="1:19" ht="89.25" x14ac:dyDescent="0.25">
@@ -4680,16 +4680,16 @@
         <v>179</v>
       </c>
       <c r="J46" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="K46" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="K46" s="3" t="s">
+      <c r="L46" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="L46" s="3" t="s">
+      <c r="M46" s="8" t="s">
         <v>386</v>
-      </c>
-      <c r="M46" s="8" t="s">
-        <v>387</v>
       </c>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
@@ -4731,17 +4731,17 @@
       <c r="H47" s="3"/>
       <c r="I47" s="8"/>
       <c r="J47" s="11" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="M47" s="8"/>
       <c r="N47" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O47" s="3"/>
       <c r="P47" s="3" t="s">
@@ -4754,7 +4754,7 @@
         <v>32</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="48" spans="1:19" ht="89.25" x14ac:dyDescent="0.25">
@@ -4782,16 +4782,16 @@
         <v>185</v>
       </c>
       <c r="J48" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="K48" s="3" t="s">
         <v>184</v>
       </c>
       <c r="L48" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="M48" s="8" t="s">
         <v>390</v>
-      </c>
-      <c r="M48" s="8" t="s">
-        <v>391</v>
       </c>
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
@@ -4833,19 +4833,19 @@
         <v>189</v>
       </c>
       <c r="J49" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="K49" s="11" t="s">
         <v>392</v>
       </c>
-      <c r="K49" s="11" t="s">
+      <c r="L49" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="L49" s="3" t="s">
+      <c r="M49" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="M49" s="8" t="s">
+      <c r="O49" s="3" t="s">
         <v>395</v>
-      </c>
-      <c r="O49" s="3" t="s">
-        <v>396</v>
       </c>
       <c r="P49" s="3" t="s">
         <v>23</v>
@@ -4857,7 +4857,7 @@
         <v>204</v>
       </c>
       <c r="S49" s="11" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="85.5" x14ac:dyDescent="0.25">
@@ -4885,20 +4885,20 @@
         <v>189</v>
       </c>
       <c r="J50" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="K50" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="K50" s="11" t="s">
+      <c r="L50" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="L50" s="3" t="s">
-        <v>400</v>
-      </c>
       <c r="M50" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N50" s="3"/>
       <c r="O50" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="P50" s="3" t="s">
         <v>23</v>
@@ -4910,7 +4910,7 @@
         <v>204</v>
       </c>
       <c r="S50" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -5028,20 +5028,20 @@
         <v>189</v>
       </c>
       <c r="J53" s="11" t="s">
+        <v>402</v>
+      </c>
+      <c r="K53" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="K53" s="3" t="s">
+      <c r="L53" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="L53" s="3" t="s">
-        <v>405</v>
-      </c>
       <c r="M53" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N53" s="3"/>
       <c r="O53" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="P53" s="3" t="s">
         <v>23</v>
@@ -5053,7 +5053,7 @@
         <v>39</v>
       </c>
       <c r="S53" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="54" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -5126,16 +5126,16 @@
         <v>189</v>
       </c>
       <c r="J55" s="11" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K55" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="M55" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N55" s="3"/>
       <c r="O55" s="3"/>
@@ -5177,16 +5177,16 @@
         <v>189</v>
       </c>
       <c r="J56" s="11" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="M56" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
@@ -5228,16 +5228,16 @@
         <v>189</v>
       </c>
       <c r="J57" s="11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="M57" s="8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="N57" s="3"/>
       <c r="O57" s="3"/>
@@ -5279,20 +5279,20 @@
         <v>189</v>
       </c>
       <c r="J58" s="11" t="s">
+        <v>407</v>
+      </c>
+      <c r="K58" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="K58" s="3" t="s">
+      <c r="L58" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="L58" s="3" t="s">
-        <v>410</v>
-      </c>
       <c r="M58" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N58" s="3"/>
       <c r="O58" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="P58" s="3" t="s">
         <v>23</v>
@@ -5304,7 +5304,7 @@
         <v>39</v>
       </c>
       <c r="S58" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
@@ -5545,19 +5545,19 @@
       <c r="H64" s="3"/>
       <c r="I64" s="8"/>
       <c r="J64" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="K64" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="K64" s="3" t="s">
+      <c r="L64" s="3" t="s">
         <v>414</v>
-      </c>
-      <c r="L64" s="3" t="s">
-        <v>415</v>
       </c>
       <c r="M64" s="8" t="s">
         <v>287</v>
       </c>
       <c r="N64" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="O64" s="3"/>
       <c r="P64" s="3" t="s">
@@ -5641,16 +5641,16 @@
         <v>228</v>
       </c>
       <c r="J66" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="K66" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="K66" s="3" t="s">
+      <c r="L66" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="L66" s="3" t="s">
-        <v>419</v>
-      </c>
       <c r="M66" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N66" s="3"/>
       <c r="O66" s="3"/>
@@ -5664,7 +5664,7 @@
         <v>39</v>
       </c>
       <c r="S66" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="67" spans="1:19" ht="142.5" x14ac:dyDescent="0.25">
@@ -5692,19 +5692,19 @@
       <c r="H67" s="3"/>
       <c r="I67" s="8"/>
       <c r="J67" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="K67" s="11" t="s">
         <v>421</v>
       </c>
-      <c r="K67" s="11" t="s">
+      <c r="L67" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="L67" s="3" t="s">
+      <c r="M67" s="8" t="s">
         <v>423</v>
       </c>
-      <c r="M67" s="8" t="s">
+      <c r="N67" s="11" t="s">
         <v>424</v>
-      </c>
-      <c r="N67" s="11" t="s">
-        <v>425</v>
       </c>
       <c r="O67" s="3"/>
       <c r="P67" s="3" t="s">
@@ -5717,7 +5717,7 @@
         <v>32</v>
       </c>
       <c r="S67" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="68" spans="1:19" ht="409.5" x14ac:dyDescent="0.25">
@@ -5745,19 +5745,19 @@
         <v>234</v>
       </c>
       <c r="J68" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="K68" s="11" t="s">
         <v>421</v>
       </c>
-      <c r="K68" s="11" t="s">
+      <c r="L68" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="L68" s="3" t="s">
+      <c r="M68" s="8" t="s">
         <v>423</v>
       </c>
-      <c r="M68" s="8" t="s">
+      <c r="N68" s="11" t="s">
         <v>424</v>
-      </c>
-      <c r="N68" s="11" t="s">
-        <v>425</v>
       </c>
       <c r="O68" s="3"/>
       <c r="P68" s="3" t="s">
@@ -5770,7 +5770,7 @@
         <v>204</v>
       </c>
       <c r="S68" s="11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="89.25" x14ac:dyDescent="0.25">
@@ -5798,16 +5798,16 @@
         <v>237</v>
       </c>
       <c r="J69" s="11" t="s">
+        <v>427</v>
+      </c>
+      <c r="K69" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="K69" s="3" t="s">
+      <c r="L69" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="L69" s="3" t="s">
+      <c r="M69" s="8" t="s">
         <v>430</v>
-      </c>
-      <c r="M69" s="8" t="s">
-        <v>431</v>
       </c>
       <c r="N69" s="3"/>
       <c r="O69" s="3"/>
@@ -5821,7 +5821,7 @@
         <v>39</v>
       </c>
       <c r="S69" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="70" spans="1:19" ht="156.75" x14ac:dyDescent="0.25">
@@ -5849,19 +5849,19 @@
         <v>240</v>
       </c>
       <c r="J70" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="K70" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="K70" s="3" t="s">
+      <c r="L70" s="3" t="s">
         <v>434</v>
-      </c>
-      <c r="L70" s="3" t="s">
-        <v>435</v>
       </c>
       <c r="M70" s="8" t="s">
         <v>287</v>
       </c>
       <c r="N70" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="O70" s="3"/>
       <c r="P70" s="3" t="s">
@@ -5874,7 +5874,7 @@
         <v>204</v>
       </c>
       <c r="S70" s="11" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="71" spans="1:19" ht="51" x14ac:dyDescent="0.25">
@@ -5992,19 +5992,19 @@
         <v>248</v>
       </c>
       <c r="J73" s="11" t="s">
+        <v>437</v>
+      </c>
+      <c r="K73" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="K73" s="3" t="s">
+      <c r="L73" s="3" t="s">
         <v>439</v>
-      </c>
-      <c r="L73" s="3" t="s">
-        <v>440</v>
       </c>
       <c r="M73" s="8" t="s">
         <v>287</v>
       </c>
       <c r="N73" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="O73" s="3"/>
       <c r="P73" s="3" t="s">
@@ -6090,19 +6090,19 @@
         <v>256</v>
       </c>
       <c r="J75" s="11" t="s">
+        <v>440</v>
+      </c>
+      <c r="K75" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="K75" s="3" t="s">
+      <c r="L75" s="3" t="s">
         <v>442</v>
-      </c>
-      <c r="L75" s="3" t="s">
-        <v>443</v>
       </c>
       <c r="M75" s="8" t="s">
         <v>287</v>
       </c>
       <c r="N75" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="O75" s="3"/>
       <c r="P75" s="3" t="s">
@@ -6115,7 +6115,7 @@
         <v>204</v>
       </c>
       <c r="S75" s="11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.25">
@@ -6324,19 +6324,19 @@
         <v>189</v>
       </c>
       <c r="J80" s="11" t="s">
+        <v>444</v>
+      </c>
+      <c r="K80" s="11" t="s">
         <v>445</v>
       </c>
-      <c r="K80" s="11" t="s">
+      <c r="L80" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="L80" s="3" t="s">
+      <c r="M80" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="N80" s="11" t="s">
         <v>447</v>
-      </c>
-      <c r="M80" s="8" t="s">
-        <v>342</v>
-      </c>
-      <c r="N80" s="11" t="s">
-        <v>448</v>
       </c>
       <c r="O80" s="3"/>
       <c r="P80" s="3" t="s">
@@ -6349,7 +6349,7 @@
         <v>204</v>
       </c>
       <c r="S80" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="81" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
@@ -6422,19 +6422,19 @@
         <v>189</v>
       </c>
       <c r="J82" s="11" t="s">
+        <v>449</v>
+      </c>
+      <c r="K82" s="11" t="s">
         <v>450</v>
       </c>
-      <c r="K82" s="11" t="s">
+      <c r="L82" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="L82" s="3" t="s">
+      <c r="M82" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="M82" s="8" t="s">
+      <c r="N82" s="11" t="s">
         <v>453</v>
-      </c>
-      <c r="N82" s="11" t="s">
-        <v>454</v>
       </c>
       <c r="O82" s="3"/>
       <c r="P82" s="3" t="s">
@@ -6447,7 +6447,7 @@
         <v>204</v>
       </c>
       <c r="S82" s="13" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>